<commit_message>
added instructions data type and control bits
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7515"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -168,6 +169,33 @@
   </si>
   <si>
     <t>Operation</t>
+  </si>
+  <si>
+    <t>RegWrite</t>
+  </si>
+  <si>
+    <t>MemtoReg</t>
+  </si>
+  <si>
+    <t>MemWrite</t>
+  </si>
+  <si>
+    <t>ALUSrc</t>
+  </si>
+  <si>
+    <t>SignExtend</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -232,6 +260,25 @@
     <tableColumn id="4" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:J17" totalsRowShown="0">
+  <autoFilter ref="A1:J17"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="10" name="Data Type"/>
+    <tableColumn id="2" name="Opcode"/>
+    <tableColumn id="3" name="Operation"/>
+    <tableColumn id="4" name="Description"/>
+    <tableColumn id="5" name="RegWrite"/>
+    <tableColumn id="6" name="MemtoReg"/>
+    <tableColumn id="7" name="MemWrite"/>
+    <tableColumn id="8" name="ALUSrc"/>
+    <tableColumn id="9" name="SignExtend"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -534,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,4 +825,345 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
circuit with  SHL,SHR, AND, OR working
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sleon\Documents\Git\computer-architecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdjoh\Documents\GitHub\computer-architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="20490" windowHeight="7515" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="20496" windowHeight="7512" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -264,8 +273,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:J17" totalsRowShown="0">
-  <autoFilter ref="A1:J17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B1:K17" totalsRowShown="0">
+  <autoFilter ref="B1:K17"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="10" name="Data Type"/>
@@ -585,15 +594,15 @@
       <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -621,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -635,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -649,7 +658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -663,7 +672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -677,7 +686,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -691,7 +700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -705,7 +714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -719,7 +728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -733,7 +742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -747,7 +756,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -761,7 +770,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -775,7 +784,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -786,7 +795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -797,7 +806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -808,7 +817,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -829,78 +838,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
       <c r="H2">
         <v>0</v>
       </c>
@@ -910,46 +922,52 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
         <v>0</v>
       </c>
@@ -959,219 +977,288 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>55</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>33</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>56</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added instruction binary and hex
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdjoh\Documents\GitHub\computer-architecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sleon\Documents\Git\computer-architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="20496" windowHeight="7512" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="20490" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Control" sheetId="2" r:id="rId2"/>
+    <sheet name="Instruction List" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -205,13 +206,97 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>OpCode</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Rd</t>
+  </si>
+  <si>
+    <t>Rs1</t>
+  </si>
+  <si>
+    <t>Rs2</t>
+  </si>
+  <si>
+    <t>Short_Offset</t>
+  </si>
+  <si>
+    <t>LD X1, #4</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>ISA</t>
+  </si>
+  <si>
+    <t>LD X2, #8</t>
+  </si>
+  <si>
+    <t>ST X1, #3</t>
+  </si>
+  <si>
+    <t>ST X2, #7</t>
+  </si>
+  <si>
+    <t>ADD X3, X1, X2</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>SUB X4, X3, X1</t>
+  </si>
+  <si>
+    <t>SHL X5, X1, X4</t>
+  </si>
+  <si>
+    <t>SHRA X6, X5, X4</t>
+  </si>
+  <si>
+    <t>AND X1, X3, X6</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>OR X2, X6, X4</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>NOT X6, #0</t>
+  </si>
+  <si>
+    <t>Long Offset</t>
+  </si>
+  <si>
+    <t>BR #2</t>
+  </si>
+  <si>
+    <t>RTS X1, #3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,13 +304,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -240,8 +351,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,15 +726,15 @@
       <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -630,7 +762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -644,7 +776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -658,7 +790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -672,7 +804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -686,7 +818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -700,7 +832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -714,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -728,7 +860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -742,7 +874,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -756,7 +888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -770,7 +902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -784,7 +916,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -795,7 +927,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -806,7 +938,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -817,7 +949,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -838,25 +970,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -891,7 +1023,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -901,7 +1033,7 @@
       <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="9">
         <v>0</v>
       </c>
       <c r="E2" t="s">
@@ -926,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -946,7 +1078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -956,7 +1088,7 @@
       <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>2</v>
       </c>
       <c r="E4" t="s">
@@ -981,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1000,8 +1132,11 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1011,7 +1146,7 @@
       <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>4</v>
       </c>
       <c r="E6" t="s">
@@ -1021,7 +1156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1031,7 +1166,7 @@
       <c r="C7" t="s">
         <v>55</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>5</v>
       </c>
       <c r="E7" t="s">
@@ -1049,8 +1184,11 @@
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1060,7 +1198,7 @@
       <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>6</v>
       </c>
       <c r="E8" t="s">
@@ -1079,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1089,7 +1227,7 @@
       <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
@@ -1099,7 +1237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1109,7 +1247,7 @@
       <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="9">
         <v>8</v>
       </c>
       <c r="E10" t="s">
@@ -1119,7 +1257,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1129,7 +1267,7 @@
       <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="9">
         <v>9</v>
       </c>
       <c r="E11" t="s">
@@ -1148,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1158,7 +1296,7 @@
       <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>10</v>
       </c>
       <c r="E12" t="s">
@@ -1177,9 +1315,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -1187,7 +1325,7 @@
       <c r="C13" t="s">
         <v>56</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <v>11</v>
       </c>
       <c r="E13" t="s">
@@ -1206,13 +1344,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
       </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
       <c r="D14">
         <v>12</v>
       </c>
@@ -1220,21 +1361,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="D15">
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="9">
         <v>13</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1248,7 +1392,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -1264,8 +1408,1884 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1">
+        <v>8</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <v>8</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1">
+        <v>3</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1">
+        <v>6</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1">
+        <v>9</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1">
+        <v>9</v>
+      </c>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B25" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1">
+        <v>4</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+    </row>
+    <row r="33" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B33" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1">
+        <v>5</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+    </row>
+    <row r="37" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B37" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1">
+        <v>2</v>
+      </c>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B41" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1">
+        <v>3</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1">
+        <v>0</v>
+      </c>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B45" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1">
+        <v>2</v>
+      </c>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+    </row>
+    <row r="49" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B49" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="Q51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1">
+        <v>4</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1">
+        <v>8</v>
+      </c>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1">
+        <v>3</v>
+      </c>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="109">
+    <mergeCell ref="B49:Q49"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="K50:Q50"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="N52:Q52"/>
+    <mergeCell ref="B45:Q45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="H46:Q46"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="N48:Q48"/>
+    <mergeCell ref="B41:Q41"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="K42:Q42"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="B37:Q37"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="B33:Q33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="B29:Q29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="B25:Q25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="B21:Q21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="B13:Q13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:Q14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:Q10"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more instructions in bin and oct
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="20490" windowHeight="7515" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -290,6 +290,15 @@
   </si>
   <si>
     <t>RTS X1, #3</t>
+  </si>
+  <si>
+    <t>ADDM X1, #0</t>
+  </si>
+  <si>
+    <t>SUBM X2, #1</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -353,16 +362,7 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,10 +370,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,9 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1033,7 +1040,7 @@
       <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="5">
         <v>0</v>
       </c>
       <c r="E2" t="s">
@@ -1068,7 +1075,7 @@
       <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -1088,7 +1095,7 @@
       <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
       <c r="E4" t="s">
@@ -1123,7 +1130,7 @@
       <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
@@ -1132,9 +1139,9 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2"/>
-      <c r="AI5" s="2"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1146,7 +1153,7 @@
       <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
       <c r="E6" t="s">
@@ -1166,7 +1173,7 @@
       <c r="C7" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="5">
         <v>5</v>
       </c>
       <c r="E7" t="s">
@@ -1184,9 +1191,9 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1198,7 +1205,7 @@
       <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="5">
         <v>6</v>
       </c>
       <c r="E8" t="s">
@@ -1227,7 +1234,7 @@
       <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="5">
         <v>7</v>
       </c>
       <c r="E9" t="s">
@@ -1247,7 +1254,7 @@
       <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="5">
         <v>8</v>
       </c>
       <c r="E10" t="s">
@@ -1267,7 +1274,7 @@
       <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="5">
         <v>9</v>
       </c>
       <c r="E11" t="s">
@@ -1296,7 +1303,7 @@
       <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>10</v>
       </c>
       <c r="E12" t="s">
@@ -1325,7 +1332,7 @@
       <c r="C13" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="5">
         <v>11</v>
       </c>
       <c r="E13" t="s">
@@ -1354,7 +1361,7 @@
       <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>12</v>
       </c>
       <c r="E14" t="s">
@@ -1371,7 +1378,7 @@
       <c r="C15" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="5">
         <v>13</v>
       </c>
       <c r="E15" t="s">
@@ -1417,62 +1424,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1531,81 +1538,81 @@
       <c r="A4" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="9">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
         <v>4</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9">
         <v>8</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1">
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9">
         <v>4</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="3" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1664,81 +1671,81 @@
       <c r="A8" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="9">
         <v>2</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9">
         <v>5</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9">
         <v>8</v>
       </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="3" t="s">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1797,81 +1804,81 @@
       <c r="A12" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="9">
         <v>2</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9">
         <v>8</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9">
         <v>8</v>
       </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9">
         <v>3</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="3" t="s">
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1930,85 +1937,85 @@
       <c r="A16" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="9">
         <v>2</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9">
         <v>9</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9">
         <v>6</v>
       </c>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="5" t="s">
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="4" t="s">
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="3" t="s">
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2067,85 +2074,85 @@
       <c r="A20" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
+      <c r="B20" s="9">
+        <v>0</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1" t="s">
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="5" t="s">
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="4" t="s">
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="3" t="s">
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2204,85 +2211,85 @@
       <c r="A24" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1">
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9">
         <v>9</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1">
-        <v>1</v>
-      </c>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1">
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9">
+        <v>1</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9">
         <v>9</v>
       </c>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="5" t="s">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="4" t="s">
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="3" t="s">
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2341,85 +2348,85 @@
       <c r="A28" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1">
+      <c r="B28" s="9">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9">
         <v>5</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1">
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9">
         <v>4</v>
       </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1" t="s">
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
     </row>
     <row r="29" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="5" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="4" t="s">
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="3" t="s">
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2478,85 +2485,85 @@
       <c r="A32" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1">
+      <c r="B32" s="9">
+        <v>1</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9">
         <v>9</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1" t="s">
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
     </row>
     <row r="33" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="5" t="s">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="4" t="s">
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="3" t="s">
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -2615,85 +2622,85 @@
       <c r="A36" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1">
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9">
         <v>5</v>
       </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1" t="s">
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="5" t="s">
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="4" t="s">
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="3" t="s">
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -2752,81 +2759,81 @@
       <c r="A40" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1" t="s">
+      <c r="B40" s="9">
+        <v>1</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1" t="s">
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1">
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9">
         <v>2</v>
       </c>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
     </row>
     <row r="41" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="4" t="s">
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="3" t="s">
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2885,79 +2892,79 @@
       <c r="A44" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="9">
         <v>2</v>
       </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9">
         <v>3</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1">
-        <v>0</v>
-      </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1">
-        <v>0</v>
-      </c>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9">
+        <v>0</v>
+      </c>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9">
+        <v>0</v>
+      </c>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
     </row>
     <row r="45" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="4" t="s">
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3016,81 +3023,81 @@
       <c r="A48" t="s">
         <v>69</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="9">
         <v>2</v>
       </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1" t="s">
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1">
-        <v>0</v>
-      </c>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1">
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9">
+        <v>0</v>
+      </c>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9">
         <v>2</v>
       </c>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
     </row>
     <row r="49" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="4" t="s">
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="3" t="s">
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -3149,48 +3156,392 @@
       <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="9">
         <v>3</v>
       </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1">
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9">
         <v>4</v>
       </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1">
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9">
         <v>8</v>
       </c>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1">
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9">
         <v>3</v>
       </c>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
+    </row>
+    <row r="53" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B53" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="9">
+        <v>0</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9">
+        <v>4</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9">
+        <v>8</v>
+      </c>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9">
+        <v>0</v>
+      </c>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
+    </row>
+    <row r="57" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B57" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
+      <c r="Q57" s="6"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="9">
+        <v>0</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9">
+        <v>0</v>
+      </c>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9">
+        <v>1</v>
+      </c>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="109">
-    <mergeCell ref="B49:Q49"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="K50:Q50"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="N52:Q52"/>
-    <mergeCell ref="B45:Q45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="H46:Q46"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="N48:Q48"/>
+  <mergeCells count="125">
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="K58:Q58"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="B53:Q53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="K54:Q54"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="N56:Q56"/>
+    <mergeCell ref="B57:Q57"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B13:Q13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:Q14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:Q10"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="B21:Q21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="B25:Q25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="B29:Q29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="B33:Q33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="N36:Q36"/>
     <mergeCell ref="B41:Q41"/>
     <mergeCell ref="D42:G42"/>
     <mergeCell ref="H42:J42"/>
@@ -3208,83 +3559,21 @@
     <mergeCell ref="F40:I40"/>
     <mergeCell ref="J40:M40"/>
     <mergeCell ref="N40:Q40"/>
-    <mergeCell ref="B33:Q33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="B29:Q29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="B25:Q25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="B21:Q21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="B13:Q13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:Q14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="B9:Q9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:Q10"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:Q2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B49:Q49"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="K50:Q50"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="N52:Q52"/>
+    <mergeCell ref="B45:Q45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="H46:Q46"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="N48:Q48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>